<commit_message>
add code for cleaning  + clean csv + variables xlsx
</commit_message>
<xml_diff>
--- a/Assignment_1/data/raw/variables_population_data.xlsx
+++ b/Assignment_1/data/raw/variables_population_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da2\Assignment_1\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69594C24-CC49-4B09-9B2A-73808DBFCB08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001A72AC-59D3-43D6-A410-9CD21E961173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="1170" windowWidth="18000" windowHeight="9360" xr2:uid="{A0F64C6D-1892-4794-993C-D0C737F0D839}"/>
+    <workbookView xWindow="25725" yWindow="1035" windowWidth="18000" windowHeight="9360" xr2:uid="{A0F64C6D-1892-4794-993C-D0C737F0D839}"/>
   </bookViews>
   <sheets>
-    <sheet name="covid_data" sheetId="1" r:id="rId1"/>
+    <sheet name="population" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>